<commit_message>
Started work on Sea Turtle
</commit_message>
<xml_diff>
--- a/Notes/Schedule.xlsx
+++ b/Notes/Schedule.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10653402\Documents\Spring_2017_Chrystel\BackUp\Fall-2018\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buhlerfamily/Desktop/Chrystel/Fall_2018/Fall-2018/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="8360" yWindow="5960" windowWidth="29760" windowHeight="17340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>10th</t>
   </si>
@@ -44,18 +50,6 @@
     <t>26th</t>
   </si>
   <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Finalize layout, start blocking  out major objects</t>
-  </si>
-  <si>
-    <t>Housekeeping! Tidy up the layout, tentively set out secondary objects</t>
-  </si>
-  <si>
     <t>Lock up Terrain, and building placements. Prepare for AI.</t>
   </si>
   <si>
@@ -66,13 +60,25 @@
   </si>
   <si>
     <t xml:space="preserve">Light concept painting, be prepared for presentations. </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Finalize layout, start blocking  out major objects.</t>
+  </si>
+  <si>
+    <t>Housekeeping! Tidy up the layout, tentively set out secondary objects.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +86,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -97,12 +116,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,78 +480,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="55.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>